<commit_message>
update.  topopoints seesm to be working correctly.  before adjusting prop change events
</commit_message>
<xml_diff>
--- a/WpfApp1-ListControlTest/Coordinate Calculations.xlsx
+++ b/WpfApp1-ListControlTest/Coordinate Calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Programming\VisualStudioProjects\WpfApp1-ListControlTest\WpfApp1-ListControlTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1903BC51-8589-445A-8AE1-7787CDBAA288}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463CE497-D2D7-4008-9432-F006C7936514}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57192" yWindow="288" windowWidth="27660" windowHeight="21900" xr2:uid="{6D7D1679-9804-4EC8-ACBA-6D68DCABFD4C}"/>
   </bookViews>
@@ -538,7 +538,7 @@
   <dimension ref="A4:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -910,14 +910,14 @@
         <v>24</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13:H13" ca="1" si="9">INDIRECT(E13)-INDIRECT(E12)</f>
+        <f t="shared" ref="F13" ca="1" si="9">INDIRECT(E13)-INDIRECT(E12)</f>
         <v>60</v>
       </c>
       <c r="G13" t="s">
         <v>25</v>
       </c>
       <c r="H13">
-        <f t="shared" ref="H13:J13" ca="1" si="10">INDIRECT(G13)-INDIRECT(G12)</f>
+        <f t="shared" ref="H13" ca="1" si="10">INDIRECT(G13)-INDIRECT(G12)</f>
         <v>60</v>
       </c>
       <c r="I13" t="s">
@@ -953,14 +953,14 @@
         <v>27</v>
       </c>
       <c r="F14">
-        <f t="shared" ref="F14:H14" ca="1" si="11">INDIRECT(E14)-INDIRECT(E13)</f>
+        <f t="shared" ref="F14" ca="1" si="11">INDIRECT(E14)-INDIRECT(E13)</f>
         <v>240</v>
       </c>
       <c r="G14" t="s">
         <v>28</v>
       </c>
       <c r="H14">
-        <f t="shared" ref="H14:J14" ca="1" si="12">INDIRECT(G14)-INDIRECT(G13)</f>
+        <f t="shared" ref="H14" ca="1" si="12">INDIRECT(G14)-INDIRECT(G13)</f>
         <v>240</v>
       </c>
       <c r="I14" t="s">
@@ -987,14 +987,14 @@
         <v>30</v>
       </c>
       <c r="F15">
-        <f t="shared" ref="F15:H15" ca="1" si="13">INDIRECT(E15)-INDIRECT(E14)</f>
+        <f t="shared" ref="F15" ca="1" si="13">INDIRECT(E15)-INDIRECT(E14)</f>
         <v>-10901</v>
       </c>
       <c r="G15" t="s">
         <v>31</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="H15:J15" ca="1" si="14">INDIRECT(G15)-INDIRECT(G14)</f>
+        <f t="shared" ref="H15" ca="1" si="14">INDIRECT(G15)-INDIRECT(G14)</f>
         <v>-20901</v>
       </c>
       <c r="I15" t="s">
@@ -1018,14 +1018,14 @@
         <v>33</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16:H16" ca="1" si="15">INDIRECT(E16)-INDIRECT(E15)</f>
+        <f t="shared" ref="F16" ca="1" si="15">INDIRECT(E16)-INDIRECT(E15)</f>
         <v>0</v>
       </c>
       <c r="G16" t="s">
         <v>34</v>
       </c>
       <c r="H16">
-        <f t="shared" ref="H16:J16" ca="1" si="16">INDIRECT(G16)-INDIRECT(G15)</f>
+        <f t="shared" ref="H16" ca="1" si="16">INDIRECT(G16)-INDIRECT(G15)</f>
         <v>0</v>
       </c>
       <c r="I16" t="s">
@@ -1049,14 +1049,14 @@
         <v>36</v>
       </c>
       <c r="F17">
-        <f t="shared" ref="F17:H17" ca="1" si="17">INDIRECT(E17)-INDIRECT(E16)</f>
+        <f t="shared" ref="F17" ca="1" si="17">INDIRECT(E17)-INDIRECT(E16)</f>
         <v>0</v>
       </c>
       <c r="G17" t="s">
         <v>37</v>
       </c>
       <c r="H17">
-        <f t="shared" ref="H17:J17" ca="1" si="18">INDIRECT(G17)-INDIRECT(G16)</f>
+        <f t="shared" ref="H17" ca="1" si="18">INDIRECT(G17)-INDIRECT(G16)</f>
         <v>0</v>
       </c>
       <c r="I17" t="s">
@@ -1080,14 +1080,14 @@
         <v>39</v>
       </c>
       <c r="F18">
-        <f t="shared" ref="F18:H18" ca="1" si="19">INDIRECT(E18)-INDIRECT(E17)</f>
+        <f t="shared" ref="F18" ca="1" si="19">INDIRECT(E18)-INDIRECT(E17)</f>
         <v>0</v>
       </c>
       <c r="G18" t="s">
         <v>40</v>
       </c>
       <c r="H18">
-        <f t="shared" ref="H18:J18" ca="1" si="20">INDIRECT(G18)-INDIRECT(G17)</f>
+        <f t="shared" ref="H18" ca="1" si="20">INDIRECT(G18)-INDIRECT(G17)</f>
         <v>0</v>
       </c>
       <c r="I18" t="s">
@@ -1111,14 +1111,14 @@
         <v>42</v>
       </c>
       <c r="F19">
-        <f t="shared" ref="F19:H19" ca="1" si="21">INDIRECT(E19)-INDIRECT(E18)</f>
+        <f t="shared" ref="F19" ca="1" si="21">INDIRECT(E19)-INDIRECT(E18)</f>
         <v>0</v>
       </c>
       <c r="G19" t="s">
         <v>43</v>
       </c>
       <c r="H19">
-        <f t="shared" ref="H19:J19" ca="1" si="22">INDIRECT(G19)-INDIRECT(G18)</f>
+        <f t="shared" ref="H19" ca="1" si="22">INDIRECT(G19)-INDIRECT(G18)</f>
         <v>0</v>
       </c>
       <c r="I19" t="s">

</xml_diff>

<commit_message>
update. working but only half changed.  about to revamp whole initialization method
</commit_message>
<xml_diff>
--- a/WpfApp1-ListControlTest/Coordinate Calculations.xlsx
+++ b/WpfApp1-ListControlTest/Coordinate Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Programming\VisualStudioProjects\WpfApp1-ListControlTest\WpfApp1-ListControlTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463CE497-D2D7-4008-9432-F006C7936514}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC806DA6-C707-4AD4-9312-9F1618A36E22}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57192" yWindow="288" windowWidth="27660" windowHeight="21900" xr2:uid="{6D7D1679-9804-4EC8-ACBA-6D68DCABFD4C}"/>
+    <workbookView xWindow="45780" yWindow="828" windowWidth="34560" windowHeight="18684" xr2:uid="{6D7D1679-9804-4EC8-ACBA-6D68DCABFD4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
topopoints working.  clean up next
</commit_message>
<xml_diff>
--- a/WpfApp1-ListControlTest/Coordinate Calculations.xlsx
+++ b/WpfApp1-ListControlTest/Coordinate Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Programming\VisualStudioProjects\WpfApp1-ListControlTest\WpfApp1-ListControlTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC806DA6-C707-4AD4-9312-9F1618A36E22}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154FABA5-2DF7-4951-B9BE-C4A26FB40340}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45780" yWindow="828" windowWidth="34560" windowHeight="18684" xr2:uid="{6D7D1679-9804-4EC8-ACBA-6D68DCABFD4C}"/>
+    <workbookView xWindow="47400" yWindow="792" windowWidth="34560" windowHeight="18684" xr2:uid="{6D7D1679-9804-4EC8-ACBA-6D68DCABFD4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
updated - cleaned - complete.  commit then merge
</commit_message>
<xml_diff>
--- a/WpfApp1-ListControlTest/Coordinate Calculations.xlsx
+++ b/WpfApp1-ListControlTest/Coordinate Calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Programming\VisualStudioProjects\WpfApp1-ListControlTest\WpfApp1-ListControlTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154FABA5-2DF7-4951-B9BE-C4A26FB40340}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53468998-11A4-4970-93AD-1E390E010881}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47400" yWindow="792" windowWidth="34560" windowHeight="18684" xr2:uid="{6D7D1679-9804-4EC8-ACBA-6D68DCABFD4C}"/>
+    <workbookView xWindow="47880" yWindow="780" windowWidth="20664" windowHeight="19416" xr2:uid="{6D7D1679-9804-4EC8-ACBA-6D68DCABFD4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -538,7 +538,7 @@
   <dimension ref="A4:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -898,42 +898,42 @@
         <v>8</v>
       </c>
       <c r="B13">
-        <v>10661</v>
+        <v>10561</v>
       </c>
       <c r="C13">
-        <v>20661</v>
+        <v>20561</v>
       </c>
       <c r="D13">
-        <v>30661</v>
+        <v>30561</v>
       </c>
       <c r="E13" t="s">
         <v>24</v>
       </c>
       <c r="F13">
         <f t="shared" ref="F13" ca="1" si="9">INDIRECT(E13)-INDIRECT(E12)</f>
-        <v>60</v>
+        <v>-40</v>
       </c>
       <c r="G13" t="s">
         <v>25</v>
       </c>
       <c r="H13">
         <f t="shared" ref="H13" ca="1" si="10">INDIRECT(G13)-INDIRECT(G12)</f>
-        <v>60</v>
+        <v>-40</v>
       </c>
       <c r="I13" t="s">
         <v>26</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="8"/>
-        <v>60</v>
+        <v>-40</v>
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="2"/>
-        <v>84.852813742385706</v>
+        <v>56.568542494923804</v>
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.70710678118654746</v>
+        <v>-0.70710678118654746</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -954,25 +954,25 @@
       </c>
       <c r="F14">
         <f t="shared" ref="F14" ca="1" si="11">INDIRECT(E14)-INDIRECT(E13)</f>
-        <v>240</v>
+        <v>340</v>
       </c>
       <c r="G14" t="s">
         <v>28</v>
       </c>
       <c r="H14">
         <f t="shared" ref="H14" ca="1" si="12">INDIRECT(G14)-INDIRECT(G13)</f>
-        <v>240</v>
+        <v>340</v>
       </c>
       <c r="I14" t="s">
         <v>29</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="8"/>
-        <v>240</v>
+        <v>340</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="2"/>
-        <v>339.41125496954282</v>
+        <v>480.83261120685233</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
update.  before revise topopoints to incorporate data controls and properties from controlpts
</commit_message>
<xml_diff>
--- a/WpfApp1-ListControlTest/Coordinate Calculations.xlsx
+++ b/WpfApp1-ListControlTest/Coordinate Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Programming\VisualStudioProjects\WpfApp1-ListControlTest\WpfApp1-ListControlTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53468998-11A4-4970-93AD-1E390E010881}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8974DF7A-FD20-4130-83FB-E0B463A0D459}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47880" yWindow="780" windowWidth="20664" windowHeight="19416" xr2:uid="{6D7D1679-9804-4EC8-ACBA-6D68DCABFD4C}"/>
+    <workbookView xWindow="48912" yWindow="588" windowWidth="29904" windowHeight="20772" xr2:uid="{6D7D1679-9804-4EC8-ACBA-6D68DCABFD4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>B5</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Slope</t>
+  </si>
+  <si>
+    <t>ΔXYZ</t>
   </si>
 </sst>
 </file>
@@ -535,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926B5F53-E625-4D7B-94F9-241F58742B40}">
-  <dimension ref="A4:P19"/>
+  <dimension ref="A4:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,9 +550,10 @@
     <col min="7" max="7" width="6.21875" customWidth="1"/>
     <col min="9" max="9" width="6.21875" customWidth="1"/>
     <col min="11" max="11" width="2.88671875" customWidth="1"/>
+    <col min="14" max="14" width="3.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="F4" s="1" t="s">
         <v>45</v>
       </c>
@@ -563,13 +567,17 @@
         <v>48</v>
       </c>
       <c r="M4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -592,7 +600,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -631,11 +639,15 @@
         <v>1555.6349186104046</v>
       </c>
       <c r="M6">
+        <f ca="1">SQRT(L6*L6+J6*J6)</f>
+        <v>1905.255888325765</v>
+      </c>
+      <c r="O6">
         <f ca="1">J6/L6</f>
         <v>0.70710678118654746</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -674,11 +686,15 @@
         <v>141.42135623730951</v>
       </c>
       <c r="M7">
-        <f t="shared" ref="M7:M19" ca="1" si="3">J7/L7</f>
+        <f t="shared" ref="M7:M15" ca="1" si="3">SQRT(L7*L7+J7*J7)</f>
+        <v>173.20508075688772</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ref="O7:O19" ca="1" si="4">J7/L7</f>
         <v>0.70710678118654746</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -709,7 +725,7 @@
         <v>19</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8" ca="1" si="4">INDIRECT(I8)-INDIRECT(I7)</f>
+        <f t="shared" ref="J8" ca="1" si="5">INDIRECT(I8)-INDIRECT(I7)</f>
         <v>100</v>
       </c>
       <c r="L8">
@@ -718,10 +734,14 @@
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="3"/>
+        <v>173.20508075688772</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ca="1" si="4"/>
         <v>0.70710678118654746</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -752,7 +772,7 @@
         <v>20</v>
       </c>
       <c r="J9">
-        <f t="shared" ref="J9" ca="1" si="5">INDIRECT(I9)-INDIRECT(I8)</f>
+        <f t="shared" ref="J9" ca="1" si="6">INDIRECT(I9)-INDIRECT(I8)</f>
         <v>130</v>
       </c>
       <c r="L9">
@@ -761,10 +781,14 @@
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="3"/>
+        <v>208.3266665599966</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ca="1" si="4"/>
         <v>0.7985836518841366</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
@@ -795,7 +819,7 @@
         <v>21</v>
       </c>
       <c r="J10">
-        <f t="shared" ref="J10" ca="1" si="6">INDIRECT(I10)-INDIRECT(I9)</f>
+        <f t="shared" ref="J10" ca="1" si="7">INDIRECT(I10)-INDIRECT(I9)</f>
         <v>120</v>
       </c>
       <c r="L10">
@@ -804,10 +828,14 @@
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="3"/>
+        <v>225.61028345356956</v>
+      </c>
+      <c r="O10">
+        <f t="shared" ca="1" si="4"/>
         <v>0.62810870710825639</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -838,7 +866,7 @@
         <v>22</v>
       </c>
       <c r="J11">
-        <f t="shared" ref="J11" ca="1" si="7">INDIRECT(I11)-INDIRECT(I10)</f>
+        <f t="shared" ref="J11" ca="1" si="8">INDIRECT(I11)-INDIRECT(I10)</f>
         <v>-50</v>
       </c>
       <c r="L11">
@@ -847,10 +875,14 @@
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="3"/>
+        <v>86.602540378443862</v>
+      </c>
+      <c r="O11">
+        <f t="shared" ca="1" si="4"/>
         <v>-0.70710678118654746</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>7</v>
       </c>
@@ -881,7 +913,7 @@
         <v>23</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="J12:J19" ca="1" si="8">INDIRECT(I12)-INDIRECT(I11)</f>
+        <f t="shared" ref="J12:J19" ca="1" si="9">INDIRECT(I12)-INDIRECT(I11)</f>
         <v>100</v>
       </c>
       <c r="L12">
@@ -890,10 +922,14 @@
       </c>
       <c r="M12">
         <f t="shared" ca="1" si="3"/>
+        <v>173.20508075688772</v>
+      </c>
+      <c r="O12">
+        <f t="shared" ca="1" si="4"/>
         <v>0.70710678118654746</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>8</v>
       </c>
@@ -910,21 +946,21 @@
         <v>24</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13" ca="1" si="9">INDIRECT(E13)-INDIRECT(E12)</f>
+        <f t="shared" ref="F13" ca="1" si="10">INDIRECT(E13)-INDIRECT(E12)</f>
         <v>-40</v>
       </c>
       <c r="G13" t="s">
         <v>25</v>
       </c>
       <c r="H13">
-        <f t="shared" ref="H13" ca="1" si="10">INDIRECT(G13)-INDIRECT(G12)</f>
+        <f t="shared" ref="H13" ca="1" si="11">INDIRECT(G13)-INDIRECT(G12)</f>
         <v>-40</v>
       </c>
       <c r="I13" t="s">
         <v>26</v>
       </c>
       <c r="J13">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>-40</v>
       </c>
       <c r="L13">
@@ -933,10 +969,14 @@
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="3"/>
+        <v>69.282032302755098</v>
+      </c>
+      <c r="O13">
+        <f t="shared" ca="1" si="4"/>
         <v>-0.70710678118654746</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>9</v>
       </c>
@@ -953,21 +993,21 @@
         <v>27</v>
       </c>
       <c r="F14">
-        <f t="shared" ref="F14" ca="1" si="11">INDIRECT(E14)-INDIRECT(E13)</f>
+        <f t="shared" ref="F14" ca="1" si="12">INDIRECT(E14)-INDIRECT(E13)</f>
         <v>340</v>
       </c>
       <c r="G14" t="s">
         <v>28</v>
       </c>
       <c r="H14">
-        <f t="shared" ref="H14" ca="1" si="12">INDIRECT(G14)-INDIRECT(G13)</f>
+        <f t="shared" ref="H14" ca="1" si="13">INDIRECT(G14)-INDIRECT(G13)</f>
         <v>340</v>
       </c>
       <c r="I14" t="s">
         <v>29</v>
       </c>
       <c r="J14">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>340</v>
       </c>
       <c r="L14">
@@ -976,10 +1016,14 @@
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="3"/>
+        <v>588.89727457341826</v>
+      </c>
+      <c r="O14">
+        <f t="shared" ca="1" si="4"/>
         <v>0.70710678118654746</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10</v>
       </c>
@@ -987,21 +1031,21 @@
         <v>30</v>
       </c>
       <c r="F15">
-        <f t="shared" ref="F15" ca="1" si="13">INDIRECT(E15)-INDIRECT(E14)</f>
+        <f t="shared" ref="F15" ca="1" si="14">INDIRECT(E15)-INDIRECT(E14)</f>
         <v>-10901</v>
       </c>
       <c r="G15" t="s">
         <v>31</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="H15" ca="1" si="14">INDIRECT(G15)-INDIRECT(G14)</f>
+        <f t="shared" ref="H15" ca="1" si="15">INDIRECT(G15)-INDIRECT(G14)</f>
         <v>-20901</v>
       </c>
       <c r="I15" t="s">
         <v>32</v>
       </c>
       <c r="J15">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>-30901</v>
       </c>
       <c r="L15">
@@ -1010,130 +1054,134 @@
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="3"/>
+        <v>38865.864238429072</v>
+      </c>
+      <c r="O15">
+        <f t="shared" ca="1" si="4"/>
         <v>-1.3108673407184217</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="E16" t="s">
         <v>33</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16" ca="1" si="15">INDIRECT(E16)-INDIRECT(E15)</f>
+        <f t="shared" ref="F16" ca="1" si="16">INDIRECT(E16)-INDIRECT(E15)</f>
         <v>0</v>
       </c>
       <c r="G16" t="s">
         <v>34</v>
       </c>
       <c r="H16">
-        <f t="shared" ref="H16" ca="1" si="16">INDIRECT(G16)-INDIRECT(G15)</f>
+        <f t="shared" ref="H16" ca="1" si="17">INDIRECT(G16)-INDIRECT(G15)</f>
         <v>0</v>
       </c>
       <c r="I16" t="s">
         <v>35</v>
       </c>
       <c r="J16">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="M16" t="e">
-        <f t="shared" ca="1" si="3"/>
+      <c r="O16" t="e">
+        <f t="shared" ca="1" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E17" t="s">
         <v>36</v>
       </c>
       <c r="F17">
-        <f t="shared" ref="F17" ca="1" si="17">INDIRECT(E17)-INDIRECT(E16)</f>
+        <f t="shared" ref="F17" ca="1" si="18">INDIRECT(E17)-INDIRECT(E16)</f>
         <v>0</v>
       </c>
       <c r="G17" t="s">
         <v>37</v>
       </c>
       <c r="H17">
-        <f t="shared" ref="H17" ca="1" si="18">INDIRECT(G17)-INDIRECT(G16)</f>
+        <f t="shared" ref="H17" ca="1" si="19">INDIRECT(G17)-INDIRECT(G16)</f>
         <v>0</v>
       </c>
       <c r="I17" t="s">
         <v>38</v>
       </c>
       <c r="J17">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="M17" t="e">
-        <f t="shared" ca="1" si="3"/>
+      <c r="O17" t="e">
+        <f t="shared" ca="1" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
         <v>39</v>
       </c>
       <c r="F18">
-        <f t="shared" ref="F18" ca="1" si="19">INDIRECT(E18)-INDIRECT(E17)</f>
+        <f t="shared" ref="F18" ca="1" si="20">INDIRECT(E18)-INDIRECT(E17)</f>
         <v>0</v>
       </c>
       <c r="G18" t="s">
         <v>40</v>
       </c>
       <c r="H18">
-        <f t="shared" ref="H18" ca="1" si="20">INDIRECT(G18)-INDIRECT(G17)</f>
+        <f t="shared" ref="H18" ca="1" si="21">INDIRECT(G18)-INDIRECT(G17)</f>
         <v>0</v>
       </c>
       <c r="I18" t="s">
         <v>41</v>
       </c>
       <c r="J18">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="M18" t="e">
-        <f t="shared" ca="1" si="3"/>
+      <c r="O18" t="e">
+        <f t="shared" ca="1" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
         <v>42</v>
       </c>
       <c r="F19">
-        <f t="shared" ref="F19" ca="1" si="21">INDIRECT(E19)-INDIRECT(E18)</f>
+        <f t="shared" ref="F19" ca="1" si="22">INDIRECT(E19)-INDIRECT(E18)</f>
         <v>0</v>
       </c>
       <c r="G19" t="s">
         <v>43</v>
       </c>
       <c r="H19">
-        <f t="shared" ref="H19" ca="1" si="22">INDIRECT(G19)-INDIRECT(G18)</f>
+        <f t="shared" ref="H19" ca="1" si="23">INDIRECT(G19)-INDIRECT(G18)</f>
         <v>0</v>
       </c>
       <c r="I19" t="s">
         <v>44</v>
       </c>
       <c r="J19">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>0</v>
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="M19" t="e">
-        <f t="shared" ca="1" si="3"/>
+      <c r="O19" t="e">
+        <f t="shared" ca="1" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>